<commit_message>
todos indentados padrao Vis
</commit_message>
<xml_diff>
--- a/Suporte-ThermoSafeSite.xlsx
+++ b/Suporte-ThermoSafeSite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="229">
   <si>
     <t>Opção A — com Docker (recomendado: 1 comando e tudo sobe)</t>
   </si>
@@ -1597,6 +1597,45 @@
   </si>
   <si>
     <t>Foi definido uma senha: Facil123@. Para o user: Paulo</t>
+  </si>
+  <si>
+    <t>Versão do Paulo Hor = Docker version 28.3.3, build 980b856</t>
+  </si>
+  <si>
+    <t>PS C:\021-Repositorios\ThermoSafe&gt; docker compose pull</t>
+  </si>
+  <si>
+    <t>time="2025-09-06T15:13:10-03:00" level=warning msg="C:\\021-Repositorios\\ThermoSafe\\docker-compose.yml: the attribute `version` is obsolete, it will be ignored, please remove it to avoid potential confusion"</t>
+  </si>
+  <si>
+    <t>[+] Pulling 33/33</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ phpmyadmin Pulled                                                                                              12.0s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ db Pulled                                                                                                      14.5s</t>
+  </si>
+  <si>
+    <t>PS C:\021-Repositorios\ThermoSafe&gt; docker compose up -d</t>
+  </si>
+  <si>
+    <t>time="2025-09-06T15:14:48-03:00" level=warning msg="C:\\021-Repositorios\\ThermoSafe\\docker-compose.yml: the attribute `version` is obsolete, it will be ignored, please remove it to avoid potential confusion"</t>
+  </si>
+  <si>
+    <t>[+] Running 4/4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ Network thermosafe_default       Created                                                                        0.0s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ Volume "thermosafe_db_data"      Created                                                                        0.0s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ Container phpmyadmin_thermosafe  Started                                                                        0.4s</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ✔ Container mysql_thermosafe       Started</t>
   </si>
 </sst>
 </file>
@@ -2076,8 +2115,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D438"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="G101" sqref="G101"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="B144" sqref="B133:B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2584,31 +2623,101 @@
         <v>213</v>
       </c>
     </row>
-    <row r="132" spans="2:2" ht="23.25">
-      <c r="B132" s="3" t="s">
+    <row r="129" spans="2:2">
+      <c r="B129" s="17" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" s="17" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" s="17" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" s="17" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2">
+      <c r="B143" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2">
+      <c r="B144" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" ht="23.25">
+      <c r="B145" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="133" spans="2:2">
-      <c r="B133" s="1"/>
-    </row>
-    <row r="134" spans="2:2">
-      <c r="B134" s="4" t="s">
+    <row r="146" spans="2:4">
+      <c r="B146" s="1"/>
+    </row>
+    <row r="147" spans="2:4">
+      <c r="B147" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="135" spans="2:2">
-      <c r="B135" s="4" t="s">
+    <row r="148" spans="2:4">
+      <c r="B148" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="136" spans="2:2">
-      <c r="B136" s="4" t="s">
+    <row r="149" spans="2:4">
+      <c r="B149" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="137" spans="2:2">
-      <c r="B137" s="4" t="s">
+    <row r="150" spans="2:4">
+      <c r="B150" s="4" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>